<commit_message>
Added more data, printing out pdpt chart sizes to csv
</commit_message>
<xml_diff>
--- a/.qasmdata/experiments/1/Dell Alienware Intel i7 8700K/redundancy.xlsx
+++ b/.qasmdata/experiments/1/Dell Alienware Intel i7 8700K/redundancy.xlsx
@@ -558,10 +558,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="0" xfId="8" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -904,10 +906,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K48"/>
+  <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -924,7 +926,7 @@
     <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -959,7 +961,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -994,7 +996,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1.1000000000000001</v>
       </c>
@@ -1029,7 +1031,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1.2</v>
       </c>
@@ -1064,7 +1066,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1.3</v>
       </c>
@@ -1099,7 +1101,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1.4</v>
       </c>
@@ -1134,7 +1136,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1.5</v>
       </c>
@@ -1169,7 +1171,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1.6</v>
       </c>
@@ -1204,7 +1206,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1.7</v>
       </c>
@@ -1239,7 +1241,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1.8</v>
       </c>
@@ -1274,7 +1276,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1.9</v>
       </c>
@@ -1309,7 +1311,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1344,7 +1346,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1.1100000000000001</v>
       </c>
@@ -1379,7 +1381,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1.1200000000000001</v>
       </c>
@@ -1414,7 +1416,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>1.1299999999999999</v>
       </c>
@@ -1449,7 +1451,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>1.1399999999999999</v>
       </c>
@@ -1483,8 +1485,14 @@
       <c r="K16">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M16" s="3">
+        <v>2</v>
+      </c>
+      <c r="N16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>1.1499999999999999</v>
       </c>
@@ -1518,8 +1526,9 @@
       <c r="K17">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M17" s="3"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>1.1599999999999999</v>
       </c>
@@ -1553,8 +1562,9 @@
       <c r="K18">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M18" s="3"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>1.17</v>
       </c>
@@ -1588,8 +1598,9 @@
       <c r="K19">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M19" s="3"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>1.18</v>
       </c>
@@ -1624,7 +1635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>1.19</v>
       </c>
@@ -1659,8 +1670,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B22">
@@ -1693,8 +1704,11 @@
       <c r="K22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M22" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>1.21</v>
       </c>
@@ -1728,8 +1742,9 @@
       <c r="K23">
         <v>11</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M23" s="3"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>1.22</v>
       </c>
@@ -1763,8 +1778,9 @@
       <c r="K24">
         <v>11</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M24" s="3"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>1.23</v>
       </c>
@@ -1798,8 +1814,9 @@
       <c r="K25">
         <v>11</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M25" s="3"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>1.24</v>
       </c>
@@ -1833,8 +1850,9 @@
       <c r="K26">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M26" s="3"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>1.25</v>
       </c>
@@ -1868,9 +1886,10 @@
       <c r="K27">
         <v>12</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+      <c r="M27" s="3"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
         <v>1.26</v>
       </c>
       <c r="B28">
@@ -1903,8 +1922,9 @@
       <c r="K28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M28" s="3"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>1.27</v>
       </c>
@@ -1939,7 +1959,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>1.28</v>
       </c>
@@ -1974,7 +1994,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>1.29</v>
       </c>
@@ -2008,8 +2028,14 @@
       <c r="K31">
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M31" s="3">
+        <v>1</v>
+      </c>
+      <c r="N31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>14</v>
       </c>
@@ -2043,6 +2069,7 @@
       <c r="K32">
         <v>1</v>
       </c>
+      <c r="M32" s="3"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
@@ -2518,7 +2545,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:K39">
+  <conditionalFormatting sqref="B2:K39 N31 N16">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>